<commit_message>
updates to research projects
</commit_message>
<xml_diff>
--- a/_data/posters.xlsx
+++ b/_data/posters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danaukes\websites\idealabasu\_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2C935585-DA0A-4A47-ABB5-07A04643550E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28D75EB2-246B-41FC-BE33-038960309486}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="28800" windowHeight="15495" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="735" yWindow="735" windowWidth="28800" windowHeight="15495" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="posters" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="38">
   <si>
     <t>assets/research-posters/2017-11-furi-symposium</t>
   </si>
@@ -128,6 +128,12 @@
   </si>
   <si>
     <t>first-author</t>
+  </si>
+  <si>
+    <t>assets/research-posters/2019-11-furi-symposium</t>
+  </si>
+  <si>
+    <t>rana-mannat</t>
   </si>
 </sst>
 </file>
@@ -971,10 +977,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="C21" sqref="C21:F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1404,6 +1410,26 @@
         <v>34</v>
       </c>
     </row>
+    <row r="22" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:S35">
     <sortCondition ref="B2:B35"/>

</xml_diff>